<commit_message>
Final Completion of project
</commit_message>
<xml_diff>
--- a/Ticket_Automation/DataBase.xlsx
+++ b/Ticket_Automation/DataBase.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IMPORTANT\Final Year Project\Ticket-Assignment-Automation\Ticket_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D756FAE-B577-4081-8848-C42D99A56230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C1131D-6EF7-4AAD-8329-8E685B59769C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="3564" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Billing</t>
   </si>
@@ -127,13 +128,31 @@
   </si>
   <si>
     <t>credited</t>
+  </si>
+  <si>
+    <t>sanjaybabu618@gmail.com</t>
+  </si>
+  <si>
+    <t>samdany454@gmail.com</t>
+  </si>
+  <si>
+    <t>prathviksambath@gmail.com</t>
+  </si>
+  <si>
+    <t>ramshankaran13@gmail.com</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>Emails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +164,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,16 +194,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,7 +494,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,4 +649,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F797C71B-D00A-4C8A-9358-729AE27B3261}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D0A853CA-5F80-412F-BF99-CB1E21A1AC0F}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{F5C38FB7-D7F7-40CD-99AA-7B330BFFE519}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{2A567E4A-A12B-4007-AC16-E194415CAFF8}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{4FB86D6B-BF9A-4ADF-905A-933BBA8314E7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Project with auto update of DB and added nupkg file for bot running purpose
</commit_message>
<xml_diff>
--- a/Ticket_Automation/DataBase.xlsx
+++ b/Ticket_Automation/DataBase.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IMPORTANT\Final Year Project\Ticket-Assignment-Automation\Ticket_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C1131D-6EF7-4AAD-8329-8E685B59769C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25153721-7AA4-43E2-9ECA-701D4F4D42A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="3564" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,108 +26,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Billing</t>
   </si>
   <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>not receiving bills</t>
+  </si>
+  <si>
+    <t>unable to pay online</t>
+  </si>
+  <si>
+    <t>not able to use the internet</t>
+  </si>
+  <si>
+    <t>slow speed</t>
+  </si>
+  <si>
     <t>temporary disconnection</t>
   </si>
   <si>
+    <t>payment done but service not restored</t>
+  </si>
+  <si>
+    <t>connection issue</t>
+  </si>
+  <si>
     <t>incorrect billing</t>
   </si>
   <si>
+    <t>payment done but not updated</t>
+  </si>
+  <si>
+    <t>router configuration</t>
+  </si>
+  <si>
+    <t>device not reachable</t>
+  </si>
+  <si>
     <t>charged daily</t>
   </si>
   <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>reg blinking</t>
+  </si>
+  <si>
     <t>separate connection</t>
   </si>
   <si>
-    <t>not receiving bills</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>unable to pay online</t>
-  </si>
-  <si>
-    <t>payment done but service not restored</t>
-  </si>
-  <si>
-    <t>payment done but not updated</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>not able to use the internet</t>
-  </si>
-  <si>
-    <t>slow speed</t>
-  </si>
-  <si>
-    <t>router configuration</t>
-  </si>
-  <si>
-    <t>reg blinking</t>
+    <t>online pay</t>
   </si>
   <si>
     <t>los light</t>
   </si>
   <si>
-    <t>connection issue</t>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>pay</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>pay online</t>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>contract states</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>pon blinking</t>
+  </si>
+  <si>
+    <t>credited</t>
   </si>
   <si>
     <t>inside shifting</t>
   </si>
   <si>
+    <t>higher billing</t>
+  </si>
+  <si>
     <t>outside shifting</t>
   </si>
   <si>
-    <t>pon blinking</t>
-  </si>
-  <si>
-    <t>Wireless</t>
-  </si>
-  <si>
-    <t>device not reachable</t>
-  </si>
-  <si>
-    <t>connection</t>
+    <t>recently</t>
   </si>
   <si>
     <t>interruption</t>
   </si>
   <si>
+    <t>product</t>
+  </si>
+  <si>
     <t>los light gets blinking</t>
   </si>
   <si>
+    <t>current user</t>
+  </si>
+  <si>
     <t>service person</t>
   </si>
   <si>
+    <t>amounts</t>
+  </si>
+  <si>
     <t>disconnection</t>
   </si>
   <si>
     <t>router</t>
   </si>
   <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>online pay</t>
-  </si>
-  <si>
-    <t>pay</t>
-  </si>
-  <si>
-    <t>pay online</t>
-  </si>
-  <si>
-    <t>money</t>
-  </si>
-  <si>
-    <t>credited</t>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>Emails</t>
   </si>
   <si>
     <t>sanjaybabu618@gmail.com</t>
@@ -140,12 +170,6 @@
   </si>
   <si>
     <t>ramshankaran13@gmail.com</t>
-  </si>
-  <si>
-    <t>TAGS</t>
-  </si>
-  <si>
-    <t>Emails</t>
   </si>
 </sst>
 </file>
@@ -194,25 +218,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,156 +516,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>23</v>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>24</v>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>25</v>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>26</v>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>27</v>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -655,62 +702,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F797C71B-D00A-4C8A-9358-729AE27B3261}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D0A853CA-5F80-412F-BF99-CB1E21A1AC0F}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{F5C38FB7-D7F7-40CD-99AA-7B330BFFE519}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{2A567E4A-A12B-4007-AC16-E194415CAFF8}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{4FB86D6B-BF9A-4ADF-905A-933BBA8314E7}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>

</xml_diff>